<commit_message>
Instagram password needed to be lowercase
</commit_message>
<xml_diff>
--- a/Usernamepasswords.xlsx
+++ b/Usernamepasswords.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Women-Coders\WOMENCODER-copy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Stripe</t>
+  </si>
+  <si>
+    <t>peoplespaceoc</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,7 +218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,21 +430,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -464,7 +467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -487,7 +490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -495,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -516,7 +519,12 @@
     <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -526,9 +534,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -538,8 +551,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Instagram password needed to be lowercase"
This reverts commit 55afdadf66c55fb4d75a8400c3973bd90f2af503.
</commit_message>
<xml_diff>
--- a/Usernamepasswords.xlsx
+++ b/Usernamepasswords.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Women-Coders\WOMENCODER-copy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Stripe</t>
-  </si>
-  <si>
-    <t>peoplespaceoc</t>
   </si>
 </sst>
 </file>
@@ -183,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,7 +215,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,21 +427,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -467,7 +464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -490,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -498,7 +495,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -519,12 +516,7 @@
     <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -534,14 +526,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -551,13 +538,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>